<commit_message>
add part 3: challenges to fairness implementation
</commit_message>
<xml_diff>
--- a/FairnessinMachineLearning(Responses).xlsx
+++ b/FairnessinMachineLearning(Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="105">
   <si>
     <t>Timestamp</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>most data is biased/unfair</t>
   </si>
   <si>
     <t>Self-taught (e.g., online courses, tutorials), Bootcamp or certification program, On-the-job learning</t>
@@ -1286,7 +1289,7 @@
     </row>
     <row r="5">
       <c r="A5" s="11">
-        <v>45791.41522967593</v>
+        <v>45792.590140381944</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>25</v>
@@ -1295,19 +1298,19 @@
         <v>26</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>28</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>32</v>
@@ -1316,28 +1319,28 @@
         <v>33</v>
       </c>
       <c r="K5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>35</v>
-      </c>
       <c r="O5" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>37</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="S5" s="12" t="s">
         <v>39</v>
@@ -1345,21 +1348,21 @@
       <c r="T5" s="13"/>
       <c r="U5" s="13"/>
       <c r="V5" s="12" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="W5" s="12" t="s">
         <v>41</v>
       </c>
       <c r="X5" s="12" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="Y5" s="14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="15">
-        <v>45792.590140381944</v>
+      <c r="A6" s="6">
+        <v>45793.0</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>25</v>
@@ -1368,19 +1371,19 @@
         <v>26</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>32</v>
@@ -1389,28 +1392,28 @@
         <v>33</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>36</v>
       </c>
       <c r="N6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="P6" s="7" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>37</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>39</v>
@@ -1418,16 +1421,16 @@
       <c r="T6" s="9"/>
       <c r="U6" s="9"/>
       <c r="V6" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="W6" s="7" t="s">
         <v>41</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="Y6" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7">
@@ -1441,7 +1444,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>28</v>
@@ -1450,10 +1453,10 @@
         <v>50</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>32</v>
@@ -1500,7 +1503,7 @@
         <v>48</v>
       </c>
       <c r="Y7" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
@@ -1511,10 +1514,10 @@
         <v>25</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>28</v>
@@ -1529,7 +1532,7 @@
         <v>56</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>45</v>
@@ -1553,7 +1556,7 @@
         <v>35</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>46</v>
@@ -1571,7 +1574,7 @@
         <v>48</v>
       </c>
       <c r="Y8" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9">
@@ -1585,7 +1588,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>28</v>
@@ -1594,10 +1597,10 @@
         <v>50</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I9" s="12" t="s">
         <v>32</v>
@@ -1644,7 +1647,7 @@
         <v>48</v>
       </c>
       <c r="Y9" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10">
@@ -1655,22 +1658,22 @@
         <v>25</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>32</v>
@@ -1709,13 +1712,13 @@
         <v>47</v>
       </c>
       <c r="W10" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="X10" s="8" t="s">
         <v>48</v>
       </c>
       <c r="Y10" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11">
@@ -1726,10 +1729,10 @@
         <v>25</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>28</v>
@@ -1741,13 +1744,13 @@
         <v>30</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K11" s="20" t="s">
         <v>35</v>
@@ -1768,7 +1771,7 @@
         <v>34</v>
       </c>
       <c r="Q11" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="R11" s="20" t="s">
         <v>38</v>
@@ -1777,16 +1780,16 @@
         <v>39</v>
       </c>
       <c r="V11" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="W11" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="X11" s="20" t="s">
         <v>42</v>
       </c>
       <c r="Y11" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
@@ -1797,10 +1800,10 @@
         <v>25</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>28</v>
@@ -1812,13 +1815,13 @@
         <v>55</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>34</v>
@@ -1827,7 +1830,7 @@
         <v>36</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N12" s="8" t="s">
         <v>36</v>
@@ -1851,13 +1854,13 @@
         <v>47</v>
       </c>
       <c r="W12" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="X12" s="8" t="s">
         <v>31</v>
       </c>
       <c r="Y12" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13">
@@ -1868,10 +1871,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>28</v>
@@ -1883,13 +1886,13 @@
         <v>55</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I13" s="23" t="s">
         <v>32</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K13" s="23" t="s">
         <v>34</v>
@@ -1924,13 +1927,13 @@
         <v>47</v>
       </c>
       <c r="W13" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="X13" s="23" t="s">
         <v>31</v>
       </c>
       <c r="Y13" s="25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14">
@@ -1947,22 +1950,22 @@
         <v>27</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>31</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>57</v>
@@ -1994,16 +1997,16 @@
       <c r="T14" s="26"/>
       <c r="U14" s="26"/>
       <c r="V14" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="W14" s="20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="X14" s="20" t="s">
         <v>31</v>
       </c>
       <c r="Y14" s="21" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Z14" s="27"/>
       <c r="AA14" s="27"/>
@@ -2023,10 +2026,10 @@
         <v>26</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F15" s="20" t="s">
         <v>50</v>
@@ -2035,13 +2038,13 @@
         <v>30</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K15" s="20" t="s">
         <v>35</v>
@@ -2071,7 +2074,7 @@
         <v>39</v>
       </c>
       <c r="V15" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="W15" s="20" t="s">
         <v>41</v>
@@ -2080,7 +2083,7 @@
         <v>42</v>
       </c>
       <c r="Y15" s="21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16">
@@ -2091,13 +2094,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>50</v>
@@ -2106,7 +2109,7 @@
         <v>30</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>31</v>
@@ -2142,7 +2145,7 @@
         <v>39</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="W16" s="8" t="s">
         <v>41</v>
@@ -2151,7 +2154,7 @@
         <v>42</v>
       </c>
       <c r="Y16" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17">
@@ -2162,19 +2165,19 @@
         <v>25</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>29</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H17" s="20" t="s">
         <v>56</v>
@@ -2222,7 +2225,7 @@
         <v>48</v>
       </c>
       <c r="Y17" s="21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18">
@@ -2239,7 +2242,7 @@
         <v>53</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="29" t="s">
         <v>50</v>
@@ -2295,7 +2298,7 @@
         <v>48</v>
       </c>
       <c r="Y18" s="32" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Z18" s="27"/>
       <c r="AA18" s="27"/>
@@ -2312,13 +2315,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F19" s="20" t="s">
         <v>50</v>
@@ -2363,7 +2366,7 @@
         <v>39</v>
       </c>
       <c r="V19" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="W19" s="20" t="s">
         <v>41</v>
@@ -2372,7 +2375,7 @@
         <v>42</v>
       </c>
       <c r="Y19" s="21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20">
@@ -2386,7 +2389,7 @@
         <v>26</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>28</v>
@@ -2401,10 +2404,10 @@
         <v>56</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>36</v>
@@ -2434,7 +2437,7 @@
         <v>39</v>
       </c>
       <c r="V20" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="W20" s="8" t="s">
         <v>41</v>
@@ -2443,7 +2446,7 @@
         <v>42</v>
       </c>
       <c r="Y20" s="17" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21">
@@ -2454,22 +2457,22 @@
         <v>25</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" s="37" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H21" s="37" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I21" s="37" t="s">
         <v>32</v>
@@ -2514,7 +2517,7 @@
         <v>48</v>
       </c>
       <c r="Y21" s="39" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Part 5: Trade off
</commit_message>
<xml_diff>
--- a/FairnessinMachineLearning(Responses).xlsx
+++ b/FairnessinMachineLearning(Responses).xlsx
@@ -142,66 +142,69 @@
     <t>No</t>
   </si>
   <si>
+    <t>Ensure both false positive and false negative rates are equal across groups</t>
+  </si>
+  <si>
+    <t>Ensure both false positive and true positive rates are equal between racial groups</t>
+  </si>
+  <si>
+    <t>Maximizing accuracy, even if fairness is reduced</t>
+  </si>
+  <si>
+    <t>embedded bias in data due to the state of the world</t>
+  </si>
+  <si>
+    <t>Bachelor’s degree (e.g., CS, DS, ML courses), Bootcamp or certification program, On-the-job learning</t>
+  </si>
+  <si>
+    <t>No — equal error rates are not enough if outcomes differ</t>
+  </si>
+  <si>
+    <t>Model Design &amp; Training</t>
+  </si>
+  <si>
+    <t>Ensure that qualified individuals of all genders are treated equally</t>
+  </si>
+  <si>
+    <t>Maximizing fairness, even at some cost to accuracy</t>
+  </si>
+  <si>
+    <t>not enough knowledge about it</t>
+  </si>
+  <si>
+    <t>1–3 years</t>
+  </si>
+  <si>
+    <t>Deployment &amp; Use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data quality and historical unfairness </t>
+  </si>
+  <si>
+    <t>Bachelor’s degree (e.g., CS, DS, ML courses), Master's or PhD-level degree</t>
+  </si>
+  <si>
+    <t>More than 6 years</t>
+  </si>
+  <si>
+    <t>I’ve handled sensitive attributes but haven’t explicitly addressed fairness</t>
+  </si>
+  <si>
+    <t>Calibration (predicted probabilities mean the same thing across groups)</t>
+  </si>
+  <si>
+    <t>disagree</t>
+  </si>
+  <si>
+    <t>Data Collection</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
     <t>Use another approach than historical income values</t>
   </si>
   <si>
-    <t>Ensure both false positive and true positive rates are equal between racial groups</t>
-  </si>
-  <si>
-    <t>Maximizing accuracy, even if fairness is reduced</t>
-  </si>
-  <si>
-    <t>embedded bias in data due to the state of the world</t>
-  </si>
-  <si>
-    <t>Bachelor’s degree (e.g., CS, DS, ML courses), Bootcamp or certification program, On-the-job learning</t>
-  </si>
-  <si>
-    <t>No — equal error rates are not enough if outcomes differ</t>
-  </si>
-  <si>
-    <t>Model Design &amp; Training</t>
-  </si>
-  <si>
-    <t>Ensure that qualified individuals of all genders are treated equally</t>
-  </si>
-  <si>
-    <t>Maximizing fairness, even at some cost to accuracy</t>
-  </si>
-  <si>
-    <t>not enough knowledge about it</t>
-  </si>
-  <si>
-    <t>1–3 years</t>
-  </si>
-  <si>
-    <t>Deployment &amp; Use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data quality and historical unfairness </t>
-  </si>
-  <si>
-    <t>Bachelor’s degree (e.g., CS, DS, ML courses), Master's or PhD-level degree</t>
-  </si>
-  <si>
-    <t>More than 6 years</t>
-  </si>
-  <si>
-    <t>I’ve handled sensitive attributes but haven’t explicitly addressed fairness</t>
-  </si>
-  <si>
-    <t>Calibration (predicted probabilities mean the same thing across groups)</t>
-  </si>
-  <si>
-    <t>disagree</t>
-  </si>
-  <si>
-    <t>Data Collection</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
     <t>most data is biased/unfair</t>
   </si>
   <si>
@@ -293,9 +296,6 @@
   </si>
   <si>
     <t>Equalized Odds (equal false positive and false negative rates across groups), Equal Opportunity (equal true positive rates across groups), Statistical Parity (equal probability of positive outcomes across groups, regardless of ground truth), Calibration (predicted probabilities mean the same thing across groups)</t>
-  </si>
-  <si>
-    <t>Ensure both false positive and false negative rates are equal across groups</t>
   </si>
   <si>
     <t>Align only the true positive rates (those who actually reoffend) across groups</t>
@@ -460,6 +460,20 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
@@ -475,20 +489,6 @@
     <border>
       <left style="thin">
         <color rgb="FF442F65"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF8F9FA"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF8F9FA"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
         <color rgb="FFF8F9FA"/>
@@ -594,13 +594,16 @@
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -612,34 +615,31 @@
     <xf borderId="4" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="7" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -657,13 +657,13 @@
     <xf borderId="5" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="7" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="6" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1128,7 +1128,7 @@
       </c>
       <c r="T2" s="9"/>
       <c r="U2" s="9"/>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="10" t="s">
         <v>40</v>
       </c>
       <c r="W2" s="7" t="s">
@@ -1137,85 +1137,85 @@
       <c r="X2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="Y2" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11">
+      <c r="A3" s="12">
         <v>45791.40033682871</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="12" t="s">
+      <c r="K3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="12" t="s">
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="W3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Y3" s="14" t="s">
+      <c r="Y3" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="15">
+      <c r="A4" s="16">
         <v>45791.41522967593</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1275,7 +1275,7 @@
       <c r="T4" s="9"/>
       <c r="U4" s="9"/>
       <c r="V4" s="7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="W4" s="7" t="s">
         <v>41</v>
@@ -1283,80 +1283,80 @@
       <c r="X4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Y4" s="11" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11">
+      <c r="A5" s="12">
         <v>45792.590140381944</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="L5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="12" t="s">
+      <c r="L5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" s="12" t="s">
+      <c r="O5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="S5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="12" t="s">
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="W5" s="12" t="s">
+      <c r="W5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="X5" s="12" t="s">
+      <c r="X5" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="Y5" s="14" t="s">
+      <c r="Y5" s="15" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1421,7 +1421,7 @@
       <c r="T6" s="9"/>
       <c r="U6" s="9"/>
       <c r="V6" s="7" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="W6" s="7" t="s">
         <v>41</v>
@@ -1429,95 +1429,95 @@
       <c r="X6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="Y6" s="10" t="s">
-        <v>60</v>
+      <c r="Y6" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11">
+      <c r="A7" s="12">
         <v>45793.5981564699</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="D7" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="12" t="s">
+      <c r="G7" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="H7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q7" s="12" t="s">
+      <c r="K7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="R7" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="S7" s="12" t="s">
+      <c r="S7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="12" t="s">
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="W7" s="12" t="s">
+      <c r="W7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="12" t="s">
+      <c r="X7" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Y7" s="14" t="s">
-        <v>64</v>
+      <c r="Y7" s="15" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="16">
+      <c r="A8" s="17">
         <v>45795.607804467596</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>28</v>
@@ -1532,7 +1532,7 @@
         <v>56</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>45</v>
@@ -1556,7 +1556,7 @@
         <v>35</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>46</v>
@@ -1573,107 +1573,107 @@
       <c r="X8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="Y8" s="17" t="s">
-        <v>69</v>
+      <c r="Y8" s="18" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="18">
+      <c r="A9" s="19">
         <v>45798.0</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="12" t="s">
+      <c r="G9" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="H9" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="K9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="P9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q9" s="12" t="s">
+      <c r="K9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="R9" s="12" t="s">
+      <c r="R9" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="S9" s="12" t="s">
+      <c r="S9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="12" t="s">
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="W9" s="12" t="s">
+      <c r="W9" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="X9" s="12" t="s">
+      <c r="X9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Y9" s="14" t="s">
-        <v>70</v>
+      <c r="Y9" s="15" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="16">
+      <c r="A10" s="17">
         <v>45799.47192658565</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>32</v>
@@ -1712,98 +1712,98 @@
         <v>47</v>
       </c>
       <c r="W10" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="X10" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="Y10" s="17" t="s">
-        <v>77</v>
+      <c r="Y10" s="18" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="19">
+      <c r="A11" s="20">
         <v>45799.47717866898</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="20" t="s">
+      <c r="C11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="J11" s="20" t="s">
+      <c r="H11" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="M11" s="20" t="s">
+      <c r="I11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="N11" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="O11" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="P11" s="20" t="s">
+      <c r="N11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Q11" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="R11" s="20" t="s">
+      <c r="Q11" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="R11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="S11" s="20" t="s">
+      <c r="S11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="V11" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="W11" s="20" t="s">
+      <c r="V11" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X11" s="20" t="s">
+      <c r="W11" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="X11" s="10" t="s">
         <v>42</v>
       </c>
       <c r="Y11" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="16">
+      <c r="A12" s="17">
         <v>45799.56511436343</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>28</v>
@@ -1815,13 +1815,13 @@
         <v>55</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>34</v>
@@ -1830,7 +1830,7 @@
         <v>36</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N12" s="8" t="s">
         <v>36</v>
@@ -1854,13 +1854,13 @@
         <v>47</v>
       </c>
       <c r="W12" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="X12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="Y12" s="17" t="s">
-        <v>88</v>
+      <c r="Y12" s="18" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="13">
@@ -1871,10 +1871,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>28</v>
@@ -1886,13 +1886,13 @@
         <v>55</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I13" s="23" t="s">
         <v>32</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K13" s="23" t="s">
         <v>34</v>
@@ -1900,7 +1900,7 @@
       <c r="L13" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="M13" s="20" t="s">
+      <c r="M13" s="10" t="s">
         <v>35</v>
       </c>
       <c r="N13" s="23" t="s">
@@ -1927,82 +1927,82 @@
         <v>47</v>
       </c>
       <c r="W13" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="X13" s="23" t="s">
         <v>31</v>
       </c>
       <c r="Y13" s="25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="19">
+      <c r="A14" s="20">
         <v>45806.65839409722</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>90</v>
+      <c r="F14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J14" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="K14" s="20" t="s">
+      <c r="J14" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L14" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="M14" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="N14" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="O14" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P14" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q14" s="20" t="s">
+      <c r="L14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q14" s="10" t="s">
         <v>37</v>
       </c>
       <c r="R14" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="S14" s="20" t="s">
+      <c r="S14" s="10" t="s">
         <v>39</v>
       </c>
       <c r="T14" s="26"/>
       <c r="U14" s="26"/>
-      <c r="V14" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="W14" s="20" t="s">
+      <c r="V14" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="W14" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="X14" s="20" t="s">
+      <c r="X14" s="10" t="s">
         <v>31</v>
       </c>
       <c r="Y14" s="21" t="s">
@@ -2016,70 +2016,70 @@
       <c r="AE14" s="27"/>
     </row>
     <row r="15">
-      <c r="A15" s="19">
+      <c r="A15" s="20">
         <v>45810.745580243056</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="20" t="s">
+      <c r="E15" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="I15" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="K15" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="L15" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="M15" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="N15" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="O15" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="P15" s="20" t="s">
+      <c r="I15" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="Q15" s="20" t="s">
+      <c r="Q15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="R15" s="20" t="s">
+      <c r="R15" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="S15" s="20" t="s">
+      <c r="S15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="V15" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="W15" s="20" t="s">
+      <c r="V15" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="W15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="X15" s="20" t="s">
+      <c r="X15" s="10" t="s">
         <v>42</v>
       </c>
       <c r="Y15" s="21" t="s">
@@ -2087,17 +2087,17 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="16">
+      <c r="A16" s="17">
         <v>45815.47702890047</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>97</v>
@@ -2108,8 +2108,8 @@
       <c r="G16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="20" t="s">
-        <v>79</v>
+      <c r="H16" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>31</v>
@@ -2145,7 +2145,7 @@
         <v>39</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="W16" s="8" t="s">
         <v>41</v>
@@ -2153,75 +2153,75 @@
       <c r="X16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="Y16" s="17" t="s">
+      <c r="Y16" s="18" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="19">
+      <c r="A17" s="20">
         <v>45815.67238391204</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="20" t="s">
+      <c r="C17" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="20" t="s">
+      <c r="E17" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="20" t="s">
+      <c r="G17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="10" t="s">
         <v>45</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L17" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="M17" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="N17" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="O17" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="P17" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q17" s="20" t="s">
+      <c r="L17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="R17" s="20" t="s">
+      <c r="R17" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="S17" s="20" t="s">
+      <c r="S17" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="V17" s="20" t="s">
+      <c r="V17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="W17" s="20" t="s">
+      <c r="W17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="X17" s="20" t="s">
+      <c r="X17" s="10" t="s">
         <v>48</v>
       </c>
       <c r="Y17" s="21" t="s">
@@ -2242,7 +2242,7 @@
         <v>53</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F18" s="29" t="s">
         <v>50</v>
@@ -2288,8 +2288,8 @@
       </c>
       <c r="T18" s="31"/>
       <c r="U18" s="31"/>
-      <c r="V18" s="29" t="s">
-        <v>40</v>
+      <c r="V18" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="W18" s="29" t="s">
         <v>41</v>
@@ -2311,67 +2311,67 @@
       <c r="A19" s="33">
         <v>45821.0</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="20" t="s">
+      <c r="C19" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="13" t="s">
         <v>55</v>
       </c>
       <c r="H19" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J19" s="20" t="s">
+      <c r="J19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="20" t="s">
+      <c r="K19" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L19" s="20" t="s">
+      <c r="L19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="M19" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="N19" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="O19" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="P19" s="20" t="s">
+      <c r="M19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P19" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="Q19" s="20" t="s">
+      <c r="Q19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="R19" s="20" t="s">
+      <c r="R19" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="S19" s="20" t="s">
+      <c r="S19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="V19" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="W19" s="20" t="s">
+      <c r="V19" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="W19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="X19" s="20" t="s">
+      <c r="X19" s="10" t="s">
         <v>42</v>
       </c>
       <c r="Y19" s="21" t="s">
@@ -2404,10 +2404,10 @@
         <v>56</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>36</v>
@@ -2437,7 +2437,7 @@
         <v>39</v>
       </c>
       <c r="V20" s="8" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="W20" s="8" t="s">
         <v>41</v>
@@ -2445,7 +2445,7 @@
       <c r="X20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="Y20" s="17" t="s">
+      <c r="Y20" s="18" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2457,19 +2457,19 @@
         <v>25</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D21" s="37" t="s">
         <v>94</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F21" s="37" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H21" s="37" t="s">
         <v>103</v>

</xml_diff>